<commit_message>
New programs added and updated existing programs
</commit_message>
<xml_diff>
--- a/registerbook.xlsx
+++ b/registerbook.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apitesting248\restAssured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A60A8E3-0611-480D-A398-A2D5B9275EF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B01FA8-98E0-475F-9DB1-0400E6DCC719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F65BF5A-167E-4864-BF75-9F943501701C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -72,7 +72,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,18 +428,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE6ADF2-B781-4E81-9930-4910A76FB4C5}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="34.61328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="35.9140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="37.76171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -476,8 +473,8 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="n">
-        <v>201.0</v>
+      <c r="E2">
+        <v>201</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -486,7 +483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -499,8 +496,8 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="n">
-        <v>201.0</v>
+      <c r="E3">
+        <v>201</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -509,7 +506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -522,8 +519,8 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="n">
-        <v>201.0</v>
+      <c r="E4">
+        <v>201</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -532,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -545,8 +542,8 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="n">
-        <v>201.0</v>
+      <c r="E5">
+        <v>201</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -555,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -568,8 +565,8 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="n">
-        <v>201.0</v>
+      <c r="E6">
+        <v>201</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -578,7 +575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -591,8 +588,8 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="n">
-        <v>201.0</v>
+      <c r="E7">
+        <v>201</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -601,7 +598,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -614,8 +611,8 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="n">
-        <v>201.0</v>
+      <c r="E8">
+        <v>201</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -624,7 +621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -637,8 +634,8 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="n">
-        <v>201.0</v>
+      <c r="E9">
+        <v>201</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -647,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -660,8 +657,8 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="n">
-        <v>201.0</v>
+      <c r="E10">
+        <v>201</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -670,7 +667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -683,8 +680,8 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="n">
-        <v>201.0</v>
+      <c r="E11">
+        <v>201</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Changes done with the programs
</commit_message>
<xml_diff>
--- a/registerbook.xlsx
+++ b/registerbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apitesting248\restAssured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B01FA8-98E0-475F-9DB1-0400E6DCC719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C158C8-0568-4483-9BD9-47477839B091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F65BF5A-167E-4864-BF75-9F943501701C}"/>
   </bookViews>
@@ -51,21 +51,21 @@
     <t>Husband</t>
   </si>
   <si>
-    <t>Status code on 06-Oct-2020-11-46-44</t>
-  </si>
-  <si>
-    <t>Content type on 06-Oct-2020-11-46-44</t>
-  </si>
-  <si>
-    <t>Response body on 06-Oct-2020-11-46-44</t>
-  </si>
-  <si>
     <t>application/json; charset=utf-8</t>
   </si>
   <si>
     <t>{
   "id": 101
 }</t>
+  </si>
+  <si>
+    <t>Status code on 15-Oct-2020-12-31-06</t>
+  </si>
+  <si>
+    <t>Content type on 15-Oct-2020-12-31-06</t>
+  </si>
+  <si>
+    <t>Response body on 15-Oct-2020-12-31-06</t>
   </si>
 </sst>
 </file>
@@ -451,13 +451,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -477,10 +477,10 @@
         <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -500,10 +500,10 @@
         <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -523,10 +523,10 @@
         <v>201</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -546,10 +546,10 @@
         <v>201</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -569,10 +569,10 @@
         <v>201</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -592,10 +592,10 @@
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -615,10 +615,10 @@
         <v>201</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -638,10 +638,10 @@
         <v>201</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -661,10 +661,10 @@
         <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -684,10 +684,10 @@
         <v>201</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>